<commit_message>
anyadido tipo y cuota recargo equivalencia
</commit_message>
<xml_diff>
--- a/data/errorImporteTotal.xlsx
+++ b/data/errorImporteTotal.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="450" yWindow="-300" windowWidth="28455" windowHeight="6690"/>
+    <workbookView xWindow="180" yWindow="1605" windowWidth="28455" windowHeight="6690"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -123,7 +123,7 @@
     <t>ENCARNA ALCUTEN ORTEGA</t>
   </si>
   <si>
-    <t>A13069</t>
+    <t>A13095</t>
   </si>
 </sst>
 </file>
@@ -587,19 +587,31 @@
         <v>34</v>
       </c>
       <c r="E2" s="1">
-        <v>80</v>
+        <v>2.13</v>
       </c>
       <c r="F2" s="1">
         <v>21</v>
       </c>
       <c r="G2" s="1">
-        <v>16.8</v>
-      </c>
-      <c r="H2" s="1">
-        <v>5.2</v>
-      </c>
-      <c r="I2" s="1">
-        <v>14.17</v>
+        <v>0.45</v>
+      </c>
+      <c r="J2" s="1">
+        <v>113.07</v>
+      </c>
+      <c r="K2" s="1">
+        <v>10</v>
+      </c>
+      <c r="L2" s="1">
+        <v>11.31</v>
+      </c>
+      <c r="O2" s="1">
+        <v>100</v>
+      </c>
+      <c r="P2" s="1">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>5</v>
       </c>
       <c r="AD2" s="2">
         <v>5102</v>

</xml_diff>